<commit_message>
file handling day 01
</commit_message>
<xml_diff>
--- a/Python/Raw_Python_Checklist.xlsx
+++ b/Python/Raw_Python_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahbub\Desktop\Data Engineering\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C446497-ECC4-4A75-A9D0-E6126A1DBFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAB3DB7-30E0-4686-84C4-60F1475A1281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Learned</t>
   </si>
@@ -495,7 +495,7 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,6 +665,15 @@
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">

</xml_diff>

<commit_message>
Modules and packages question
</commit_message>
<xml_diff>
--- a/Python/Raw_Python_Checklist.xlsx
+++ b/Python/Raw_Python_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahbub\Desktop\Data Engineering\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAB3DB7-30E0-4686-84C4-60F1475A1281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B974B24-3468-4F64-9941-AA13A82B51B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
   <si>
     <t>Learned</t>
   </si>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,6 +682,15 @@
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">

</xml_diff>